<commit_message>
Nomainīts vārds darba gaitā
</commit_message>
<xml_diff>
--- a/docs/gaita.xlsx
+++ b/docs/gaita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilgvars.rocans\Documents\P-R-O-G-R-A-M\test-reader\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC5FE74-5374-4DE3-AB45-B0BEEE3FE880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F5461B-D9C5-468A-9D78-FF5AAAC4AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="924" yWindow="0" windowWidth="18192" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>Izveidot sistēmu, kas attēlos var noteikt papīra lapas stūru novietojumu</t>
   </si>
   <si>
-    <t>Izveidot sistēmu, ar ko var vērtēt pārbaudes darbus, izmantojot to pareizo atbilžu izkārtojumus un nobildētos pārbaudes darbus</t>
-  </si>
-  <si>
     <t>Izveidot attēlu pārveidošanas sistēmu, kas papīra lapu fotogrāfijas pārveido, lai lapas būtu taisnstūrveida un vertikālas attēlos</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Sagatavot programmu prezentēšanai</t>
+  </si>
+  <si>
+    <t>Izveidot sistēmu, ar ko var vērtēt pārbaudes darbus, izmantojot to pareizo atbilžu izkārtojumus un noskenētos pārbaudes darbus</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -490,7 +490,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
@@ -501,7 +501,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -512,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
i dont even know man
</commit_message>
<xml_diff>
--- a/docs/gaita.xlsx
+++ b/docs/gaita.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilgvars.rocans\Documents\P-R-O-G-R-A-M\test-reader\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F5461B-D9C5-468A-9D78-FF5AAAC4AFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018F1B24-D384-4AB5-BEB3-AFF0CE97DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="924" yWindow="0" windowWidth="18192" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,13 +72,13 @@
     <t>Izveidot sistēmu, kas ļauj fotogrāfijās no krāsām noteikt, kur uz lapas ir tukšums un kur - izdrukāti vai uzrakstīti laukumi</t>
   </si>
   <si>
-    <t>Aicināt skolotājus testēt programmu</t>
-  </si>
-  <si>
     <t>Sagatavot programmu prezentēšanai</t>
   </si>
   <si>
     <t>Izveidot sistēmu, ar ko var vērtēt pārbaudes darbus, izmantojot to pareizo atbilžu izkārtojumus un noskenētos pārbaudes darbus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Izveidot izmēģinājuma pārbaudes darbus testēšanai, prasīt skolēniem tos aizpildīt un noskenēt un nobildēt un noteikt vai </t>
   </si>
 </sst>
 </file>
@@ -399,12 +399,12 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.109375" customWidth="1"/>
+    <col min="2" max="2" width="105.109375" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -457,7 +457,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -512,7 +512,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>

</xml_diff>